<commit_message>
fixed numbering mistake in hits_map_name.xlsx
</commit_message>
<xml_diff>
--- a/hits_map_name.xlsx
+++ b/hits_map_name.xlsx
@@ -799,8 +799,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -839,7 +839,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
@@ -860,7 +860,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -881,7 +881,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
@@ -902,7 +902,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>12</v>
@@ -923,7 +923,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>16</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>20</v>
@@ -965,7 +965,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>24</v>
@@ -986,7 +986,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>28</v>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>32</v>
@@ -1028,7 +1028,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>36</v>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>40</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>44</v>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>47</v>
@@ -1146,7 +1146,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>53</v>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>59</v>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>65</v>
@@ -1221,7 +1221,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>70</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>75</v>
@@ -1267,7 +1267,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>80</v>
@@ -1290,7 +1290,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>85</v>
@@ -1313,7 +1313,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>90</v>
@@ -1336,7 +1336,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>95</v>
@@ -1359,7 +1359,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>100</v>
@@ -1380,7 +1380,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>105</v>
@@ -1402,6 +1402,7 @@
       <c r="I31" s="2"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>